<commit_message>
Checklist version 1 #44
</commit_message>
<xml_diff>
--- a/Documentatie/checklist project.xlsx
+++ b/Documentatie/checklist project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vivesonline-my.sharepoint.com/personal/r0995990_student_vives_be/Documents/Bureaublad/Vives/2024-2025/Projectjes/semmie1/GreenhouseSensoring/Documentatie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{028C025A-0B7F-44DA-BFDB-8DB6F6A28827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DFF0C4B-4327-4BC1-B4E5-A08B277FC644}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="13_ncr:1_{028C025A-0B7F-44DA-BFDB-8DB6F6A28827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA955D67-D3F7-4A36-BEED-E17261FE3D23}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24E357F3-3B44-4F45-8877-6ADD41F87A90}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="65">
   <si>
     <t>Checklist</t>
   </si>
@@ -116,14 +116,128 @@
     <t>Meettoestel</t>
   </si>
   <si>
-    <t>**:**</t>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>ESP</t>
+  </si>
+  <si>
+    <t>Multimeter</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>3V3</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
+    <t>D17</t>
+  </si>
+  <si>
+    <t>D21</t>
+  </si>
+  <si>
+    <t>RX0</t>
+  </si>
+  <si>
+    <t>TX0</t>
+  </si>
+  <si>
+    <t>D22</t>
+  </si>
+  <si>
+    <t>Avcc</t>
+  </si>
+  <si>
+    <t>LS1</t>
+  </si>
+  <si>
+    <t>Ascl</t>
+  </si>
+  <si>
+    <t>Asda</t>
+  </si>
+  <si>
+    <t>Agnd</t>
+  </si>
+  <si>
+    <t>Bvcc</t>
+  </si>
+  <si>
+    <t>Bgnd</t>
+  </si>
+  <si>
+    <t>LS2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>gnd</t>
+  </si>
+  <si>
+    <t>Osciloscoop</t>
+  </si>
+  <si>
+    <t>1bit</t>
+  </si>
+  <si>
+    <t>7bit</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>LS2 Bscl</t>
+  </si>
+  <si>
+    <t>LS2 Bsda</t>
+  </si>
+  <si>
+    <t>LS1 Bscl</t>
+  </si>
+  <si>
+    <t>LS1 Bsda</t>
+  </si>
+  <si>
+    <t>TTLRS Di</t>
+  </si>
+  <si>
+    <t>TTLRS Ro</t>
+  </si>
+  <si>
+    <t>TTLRS De &amp; Re</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,13 +269,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -174,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,11 +296,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor theme="6" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -256,12 +370,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -284,19 +427,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -305,8 +454,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
+  <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
@@ -323,6 +471,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -338,6 +507,27 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -352,7 +542,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -367,7 +577,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -382,7 +612,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -397,7 +647,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -412,7 +682,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -432,11 +722,25 @@
         <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -451,6 +755,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -465,7 +791,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -480,6 +828,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -494,6 +864,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -573,10 +965,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E914437D-CF03-4AF8-B704-83108FCC6046}" name="Tabel1" displayName="Tabel1" ref="B7:N47" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="B7:N47" xr:uid="{E914437D-CF03-4AF8-B704-83108FCC6046}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:M32">
-    <sortCondition ref="B7:B32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E914437D-CF03-4AF8-B704-83108FCC6046}" name="Tabel1" displayName="Tabel1" ref="B7:N35" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="B7:N35" xr:uid="{E914437D-CF03-4AF8-B704-83108FCC6046}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:N35">
+    <sortCondition ref="B7:B35"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="12" xr3:uid="{5AF8DDC5-A963-4C7D-9E46-77900070F275}" name="Nummer" dataDxfId="12"/>
@@ -914,10 +1306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5190BFB3-EE5C-4CCB-9A0B-7CF5215BDAAD}">
-  <dimension ref="B1:N53"/>
+  <dimension ref="B1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,8 +1341,8 @@
       <c r="C2" s="8">
         <v>45617</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>26</v>
+      <c r="D2" s="9">
+        <v>0.64166666666666672</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="31.5" x14ac:dyDescent="0.5">
@@ -973,16 +1365,16 @@
       <c r="G5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18" t="s">
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="19"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="21"/>
       <c r="N5" s="11" t="s">
         <v>20</v>
       </c>
@@ -1004,13 +1396,13 @@
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="13" t="s">
         <v>2</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1045,700 +1437,792 @@
       <c r="B8" s="12">
         <v>1</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
+      <c r="C8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15">
+        <v>5</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="18"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
         <v>2</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
+      <c r="C9" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17">
+        <v>0</v>
+      </c>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="12">
         <v>3</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
+      <c r="C10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="18"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
         <v>4</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
+      <c r="C11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17">
+        <v>3.3</v>
+      </c>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="19"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
         <v>5</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
+      <c r="C12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="18"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
         <v>6</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
+      <c r="C13" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="17">
+        <v>0</v>
+      </c>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17">
+        <v>3</v>
+      </c>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="19"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="12">
         <v>7</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
+      <c r="C14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="18"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="12">
         <v>8</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
+      <c r="C15" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="19"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="12">
         <v>9</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
+      <c r="C16" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="18"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="12">
         <v>10</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
+      <c r="C17" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="19"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="12">
         <v>11</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
+      <c r="C18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="18"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="12">
         <v>12</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
+      <c r="C19" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="19"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="12">
         <v>13</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
+      <c r="C20" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15">
+        <v>5</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="18"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="12">
         <v>14</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
+      <c r="C21" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="19"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="12">
         <v>15</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
+      <c r="C22" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="18"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>16</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
+      <c r="C23" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17">
+        <v>0</v>
+      </c>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="19"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>17</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
+      <c r="C24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15">
+        <v>3.3</v>
+      </c>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="18"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>18</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
+      <c r="C25" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17">
+        <v>0</v>
+      </c>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="19"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="12">
         <v>19</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
+      <c r="C26" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15">
+        <v>5</v>
+      </c>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="18"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="12">
         <v>20</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
+      <c r="C27" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="19"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="12">
         <v>21</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
+      <c r="C28" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="18"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="12">
         <v>22</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
+      <c r="C29" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17">
+        <v>0</v>
+      </c>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="19"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="12">
         <v>23</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
+      <c r="C30" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="14"/>
+      <c r="E30" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15">
+        <v>3.3</v>
+      </c>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="18"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="12">
         <v>24</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
+      <c r="C31" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17">
+        <v>0</v>
+      </c>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="19"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="12">
         <v>25</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
+      <c r="C32" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="14"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="18"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="12">
         <v>26</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
+      <c r="C33" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="16"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="19"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="12">
         <v>27</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
+      <c r="C34" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="14"/>
+      <c r="E34" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15">
+        <v>5</v>
+      </c>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
       <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
+      <c r="N34" s="18"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="12">
         <v>28</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="12">
+      <c r="C35" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="16"/>
+      <c r="E35" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="12">
-        <v>30</v>
-      </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="12">
-        <v>31</v>
-      </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17">
+        <v>0</v>
+      </c>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="19"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="12">
-        <v>32</v>
-      </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="12">
-        <v>33</v>
-      </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="12">
-        <v>34</v>
-      </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="12">
-        <v>35</v>
-      </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="12">
-        <v>36</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="12"/>
-      <c r="M43" s="13"/>
-      <c r="N43" s="13"/>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="12">
-        <v>37</v>
-      </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="12"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="12">
-        <v>38</v>
-      </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="13"/>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="12">
-        <v>39</v>
-      </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="12"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="12">
-        <v>40</v>
-      </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="12"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>16</v>
-      </c>
-      <c r="C52" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="B41" t="s">
         <v>18</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C41" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1747,7 +2231,7 @@
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>